<commit_message>
open a few excels and probably just changed the selected cell :S
</commit_message>
<xml_diff>
--- a/raw_data/2024_Anfrage/extracted_data/Beilage_13_14_15_16/Beilage_13_14_15_16_manually_extracted.xlsx
+++ b/raw_data/2024_Anfrage/extracted_data/Beilage_13_14_15_16/Beilage_13_14_15_16_manually_extracted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\WU\WARRA\raw_data\extracted_data\Beilage_13_14_15_16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\WU\WARRA\raw_data\2024_Anfrage\extracted_data\Beilage_13_14_15_16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E047C429-3912-4471-97C9-8EE11CC6ABF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A96FD4F-D232-4E7A-9246-C260E688CAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{012DACB6-C690-4DFD-82A2-86181B8812D4}"/>
+    <workbookView xWindow="-6360" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{012DACB6-C690-4DFD-82A2-86181B8812D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Beilage_13" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -21287,7 +21287,7 @@
   <dimension ref="A1:M319"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21297,7 +21297,7 @@
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="45.140625" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>